<commit_message>
Improved user input calls for get_classes_subbed
User input calls are now cleaner and easier to  understand. They will also show you your current progess each time you get the option to add another class.
</commit_message>
<xml_diff>
--- a/paysheetgino.xlsx
+++ b/paysheetgino.xlsx
@@ -352,7 +352,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -996,32 +996,32 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/13</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>w57</t>
+          <t>w34</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/13</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>w75</t>
+          <t>w34</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>w48</t>
+          <t>w57</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>w45</t>
+          <t>w75</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1065,12 +1065,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w48</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1080,44 +1080,44 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w45</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>w60</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>w61</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
@@ -1129,12 +1129,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>w60</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>w71</t>
+          <t>w61</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1161,12 +1161,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>w66</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1176,12 +1176,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>w71</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1193,12 +1193,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>w49</t>
+          <t>w66</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1225,59 +1225,59 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w49</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>f70</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>4/17</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
           <t>4/19</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>w67</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>4/19</t>
-        </is>
-      </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>w52</t>
+          <t>f70</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>w67</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1304,12 +1304,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w52</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1321,12 +1321,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1336,12 +1336,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Meeting</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
@@ -1353,22 +1353,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>w34</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>.5</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>w57</t>
+          <t>Meeting</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1385,22 +1385,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>w57</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>4/22</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>w75</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>4/22</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>w48</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1417,27 +1417,27 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>w48</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>4/22</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
           <t>w45</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>4/22</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>ext</t>
-        </is>
-      </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1459,17 +1459,17 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>w60</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
@@ -1481,27 +1481,27 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>w60</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>4/24</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
           <t>w61</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>4/24</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>pe</t>
-        </is>
-      </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1513,22 +1513,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>pe</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>4/24</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
           <t>w71</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>4/24</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>w66</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -1545,27 +1545,27 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>w66</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>4/24</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
           <t>pe</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>.5</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>4/24</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>w49</t>
-        </is>
-      </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
@@ -1577,12 +1577,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w49</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1604,32 +1604,32 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>4/24</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
           <t>4/26</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>f70</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>2</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>4/26</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>w67</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>1</t>
         </is>
       </c>
     </row>
@@ -1641,22 +1641,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>w67</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>4/26</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
           <t>w52</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>4/26</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>w46</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -1673,12 +1673,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1700,27 +1700,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>4/26</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
           <t>4/29</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>w57</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>w75</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -1737,22 +1737,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>w75</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>4/29</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
           <t>w48</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>w45</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -1769,12 +1769,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w45</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1788,6 +1788,23 @@
         </is>
       </c>
       <c r="H46" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>4/29</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
         <is>
           <t>.5</t>
         </is>

</xml_diff>

<commit_message>
Implement checks of some user input
Starts buiilding the checks on user input to make sure its useful. Repromts users to try again if it isn't.
</commit_message>
<xml_diff>
--- a/paysheetgino.xlsx
+++ b/paysheetgino.xlsx
@@ -352,7 +352,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,29 +659,29 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>4/5</t>
+          <t>4/8</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>f70</t>
+          <t>w57</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4/5</t>
+          <t>4/8</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>w67</t>
+          <t>w75</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -691,12 +691,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>4/5</t>
+          <t>4/8</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>w52</t>
+          <t>w48</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -708,12 +708,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4/5</t>
+          <t>4/8</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>w45</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>4/5</t>
+          <t>4/8</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -740,7 +740,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4/5</t>
+          <t>4/8</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -755,12 +755,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>w57</t>
+          <t>w60</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -772,12 +772,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>w75</t>
+          <t>w61</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -787,29 +787,29 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>w48</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>w45</t>
+          <t>w71</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -819,29 +819,29 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w66</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -856,12 +856,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>w60</t>
+          <t>w49</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -873,12 +873,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>w61</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -888,7 +888,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -900,27 +900,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>w71</t>
+          <t>f70</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>w66</t>
+          <t>w67</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -932,39 +932,39 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>w52</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>w49</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -979,7 +979,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -996,27 +996,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>f70</t>
+          <t>w57</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>w67</t>
+          <t>w75</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1028,12 +1028,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>w52</t>
+          <t>w48</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1043,12 +1043,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>w45</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1060,7 +1060,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1092,12 +1092,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>w57</t>
+          <t>w60</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1107,12 +1107,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>w75</t>
+          <t>w61</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1124,27 +1124,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>w48</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>w45</t>
+          <t>w71</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1156,27 +1156,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w66</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1193,12 +1193,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>w60</t>
+          <t>w49</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1208,12 +1208,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>w61</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1235,29 +1235,29 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>w71</t>
+          <t>f70</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>w66</t>
+          <t>w67</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1267,39 +1267,39 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>w52</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>w49</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1316,7 +1316,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1331,29 +1331,29 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>f70</t>
+          <t>w57</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>w67</t>
+          <t>w75</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1363,12 +1363,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>w52</t>
+          <t>w48</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1380,12 +1380,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>w45</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1395,7 +1395,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1412,7 +1412,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1427,12 +1427,12 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>w57</t>
+          <t>w60</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1444,12 +1444,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>w75</t>
+          <t>w61</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1459,29 +1459,29 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>w48</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>w45</t>
+          <t>w71</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1491,29 +1491,29 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w66</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1528,12 +1528,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>w60</t>
+          <t>w49</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1545,12 +1545,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>w61</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1560,7 +1560,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -1572,27 +1572,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>w71</t>
+          <t>f70</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>w66</t>
+          <t>w67</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -1604,39 +1604,39 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>w52</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>w49</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -1668,27 +1668,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>f70</t>
+          <t>w57</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>w67</t>
+          <t>w75</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -1700,12 +1700,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>w52</t>
+          <t>w48</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1715,12 +1715,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>w45</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -1732,7 +1732,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -1756,102 +1756,6 @@
         </is>
       </c>
       <c r="H45" t="inlineStr">
-        <is>
-          <t>.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>w57</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>w75</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>w48</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>w45</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>ext</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>.5</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>ext</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
         <is>
           <t>.5</t>
         </is>

</xml_diff>

<commit_message>
Changes to user_info and user_objects
User information is now saved in subdirectories via pickle.

User names, and passwords go to user_info

User objects containing the users schedule end up in user_objects.
</commit_message>
<xml_diff>
--- a/paysheetgino.xlsx
+++ b/paysheetgino.xlsx
@@ -352,7 +352,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,29 +659,29 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/5</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>w57</t>
+          <t>f70</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/5</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>w75</t>
+          <t>w67</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -691,12 +691,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/5</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>w48</t>
+          <t>w52</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -708,12 +708,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/5</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>w45</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>4/5</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -740,27 +740,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>4/5</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>4/8</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>ext</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>.5</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>4/10</t>
-        </is>
-      </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>w60</t>
+          <t>w57</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -772,12 +772,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/8</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>w61</t>
+          <t>w75</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -787,29 +787,29 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/8</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>w48</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/8</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>w71</t>
+          <t>w45</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -819,49 +819,49 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/8</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>w66</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>4/8</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>4/10</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>pe</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>.5</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>4/10</t>
-        </is>
-      </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>w49</t>
+          <t>w60</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -873,12 +873,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w61</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -888,7 +888,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -900,27 +900,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>f70</t>
+          <t>w71</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>w67</t>
+          <t>w66</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -932,39 +932,39 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>w52</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>w49</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -979,7 +979,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/10</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -996,27 +996,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>w57</t>
+          <t>f70</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>w75</t>
+          <t>w67</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1028,12 +1028,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>w48</t>
+          <t>w52</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1043,12 +1043,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>w45</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1060,7 +1060,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1092,12 +1092,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>w60</t>
+          <t>w57</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1107,12 +1107,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>w61</t>
+          <t>w75</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1124,27 +1124,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>w48</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>w71</t>
+          <t>w45</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1156,27 +1156,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>w66</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1193,12 +1193,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>w49</t>
+          <t>w60</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1208,12 +1208,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w61</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1235,29 +1235,29 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>f70</t>
+          <t>w71</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>w67</t>
+          <t>w66</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1267,39 +1267,39 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>w52</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>w49</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1316,44 +1316,44 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>4/17</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
           <t>4/19</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>ext</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>.5</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>4/22</t>
-        </is>
-      </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>w57</t>
+          <t>f70</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>w75</t>
+          <t>w67</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1363,12 +1363,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>w48</t>
+          <t>w52</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1380,12 +1380,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>w45</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1395,7 +1395,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1412,27 +1412,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>4/19</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
           <t>4/22</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>ext</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>.5</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>4/24</t>
-        </is>
-      </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>w60</t>
+          <t>w57</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1444,12 +1444,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>w61</t>
+          <t>w75</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1459,29 +1459,29 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>w48</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>w71</t>
+          <t>w45</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1491,49 +1491,49 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>w66</t>
+          <t>ext</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>4/22</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
           <t>4/24</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>pe</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>.5</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>4/24</t>
-        </is>
-      </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>w49</t>
+          <t>w60</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1545,12 +1545,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>w61</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1560,7 +1560,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>ext</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -1572,27 +1572,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>f70</t>
+          <t>w71</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>w67</t>
+          <t>w66</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -1604,39 +1604,39 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>w52</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.5</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>w49</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -1668,27 +1668,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>4/29</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>w57</t>
+          <t>f70</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>4/29</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>w75</t>
+          <t>w67</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -1700,12 +1700,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>4/29</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>w48</t>
+          <t>w52</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1715,12 +1715,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>4/29</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>w45</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -1732,30 +1732,126 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>4/26</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>4/26</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>4/29</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>ext</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>.5</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>w57</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
         <is>
           <t>4/29</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>ext</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>w75</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>4/29</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>w48</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>4/29</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>w45</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>4/29</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>4/29</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>ext</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
         <is>
           <t>.5</t>
         </is>

</xml_diff>